<commit_message>
Final upload of sprint 2 backlog
FInal breakdown and analysis of sprint 2 tasks
</commit_message>
<xml_diff>
--- a/Sprint_2_Backlog.xlsx
+++ b/Sprint_2_Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lachl\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FD5016E-7508-47A0-B8E4-EECC4C4C399C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34533290-6601-436D-B895-7B03875656B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="76">
   <si>
     <t>Story</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>As a user I would like to see the current state of the quiz</t>
-  </si>
-  <si>
-    <t>Create functionality on front end</t>
   </si>
   <si>
     <t>As a user I would like to be able to host a multiplayer quiz</t>
@@ -237,12 +234,42 @@
   <si>
     <t xml:space="preserve">Lachlan </t>
   </si>
+  <si>
+    <t>AS A user I would like to have a buffer page between each question so I can check what is happening with the quiz</t>
+  </si>
+  <si>
+    <t>Implement Design of page</t>
+  </si>
+  <si>
+    <t>Create join page</t>
+  </si>
+  <si>
+    <t>Create working lobby for host with start game functionality</t>
+  </si>
+  <si>
+    <t>Mikhail</t>
+  </si>
+  <si>
+    <t>Rauf,Robert</t>
+  </si>
+  <si>
+    <t>Alek</t>
+  </si>
+  <si>
+    <t>Rauf , Robert</t>
+  </si>
+  <si>
+    <t>As a user I can see my score between Questions</t>
+  </si>
+  <si>
+    <t>Matt, mikhail</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,8 +285,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,8 +318,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -302,12 +348,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -349,6 +424,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -358,12 +439,64 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -497,19 +630,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>40</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>33</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -546,7 +679,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>46</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1726,10 +1859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N1224"/>
+  <dimension ref="A1:GT1227"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1742,27 +1875,28 @@
     <col min="6" max="6" width="2.7109375" style="2" customWidth="1"/>
     <col min="12" max="12" width="2.7109375" style="2" customWidth="1"/>
     <col min="13" max="13" width="17.7109375" customWidth="1"/>
+    <col min="14" max="202" width="9.140625" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16"/>
       <c r="B1" s="16"/>
       <c r="C1" s="17"/>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="26" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="11"/>
       <c r="F1" s="11"/>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
       <c r="L1" s="11"/>
       <c r="M1" s="19"/>
-      <c r="N1" s="10"/>
+      <c r="N1" s="21"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
@@ -1774,7 +1908,7 @@
       <c r="C2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="24"/>
+      <c r="D2" s="26"/>
       <c r="E2" s="11" t="s">
         <v>15</v>
       </c>
@@ -1798,25 +1932,33 @@
       <c r="M2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="10"/>
+      <c r="N2" s="21"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="23" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="9"/>
+      <c r="C3" s="9">
+        <v>3</v>
+      </c>
       <c r="D3" s="9">
-        <f t="shared" ref="D3:D67" si="0">C3 - SUM(G3:K3)</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="10"/>
+        <f t="shared" ref="D3:D70" si="0">C3 - SUM(G3:K3)</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>55</v>
+      </c>
       <c r="F3" s="11"/>
       <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
+      <c r="H3" s="10">
+        <v>2</v>
+      </c>
+      <c r="I3" s="10">
+        <v>1</v>
+      </c>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
       <c r="L3" s="11"/>
@@ -1824,88 +1966,112 @@
         <f>IF(D3 = 0,"Yes","No")</f>
         <v>Yes</v>
       </c>
-      <c r="N3" s="10"/>
+      <c r="N3" s="21"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="9">
+        <v>4</v>
+      </c>
       <c r="D4" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E4" s="10"/>
+      <c r="E4" s="10" t="s">
+        <v>70</v>
+      </c>
       <c r="F4" s="11"/>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
+      <c r="J4" s="10">
+        <v>2</v>
+      </c>
+      <c r="K4" s="10">
+        <v>2</v>
+      </c>
       <c r="L4" s="11"/>
       <c r="M4" s="18" t="str">
         <f>IF(D4 = 0,"Yes","No")</f>
         <v>Yes</v>
       </c>
-      <c r="N4" s="10"/>
+      <c r="N4" s="21"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="23" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="9"/>
+      <c r="C5" s="9">
+        <v>4</v>
+      </c>
       <c r="D5" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E5" s="10"/>
+      <c r="E5" s="10" t="s">
+        <v>71</v>
+      </c>
       <c r="F5" s="11"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
+      <c r="J5" s="10">
+        <v>3</v>
+      </c>
+      <c r="K5" s="10">
+        <v>1</v>
+      </c>
       <c r="L5" s="11"/>
       <c r="M5" s="18" t="str">
-        <f t="shared" ref="M5:M69" si="1">IF(D5 = 0,"Yes","No")</f>
-        <v>Yes</v>
-      </c>
-      <c r="N5" s="10"/>
+        <f t="shared" ref="M5:M72" si="1">IF(D5 = 0,"Yes","No")</f>
+        <v>Yes</v>
+      </c>
+      <c r="N5" s="21"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="23" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="9"/>
+        <v>69</v>
+      </c>
+      <c r="C6" s="9">
+        <v>4</v>
+      </c>
       <c r="D6" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E6" s="10"/>
+      <c r="E6" s="21" t="s">
+        <v>71</v>
+      </c>
       <c r="F6" s="11"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
+      <c r="J6" s="10">
+        <v>2</v>
+      </c>
+      <c r="K6" s="10">
+        <v>2</v>
+      </c>
       <c r="L6" s="11"/>
       <c r="M6" s="18" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="N6" s="10"/>
+      <c r="N6" s="21"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" s="9">
         <v>2</v>
@@ -1915,7 +2081,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="10">
@@ -1930,82 +2096,112 @@
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="N7" s="10"/>
+      <c r="N7" s="21"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
+        <v>57</v>
+      </c>
+      <c r="C8" s="9">
+        <v>4</v>
+      </c>
+      <c r="D8" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="F8" s="11"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
+      <c r="J8" s="10">
+        <v>2</v>
+      </c>
+      <c r="K8" s="10">
+        <v>2</v>
+      </c>
       <c r="L8" s="11"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="10"/>
+      <c r="M8" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="N8" s="21"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
-        <v>22</v>
+      <c r="A9" s="23" t="s">
+        <v>21</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="9"/>
+        <v>49</v>
+      </c>
+      <c r="C9" s="9">
+        <v>3</v>
+      </c>
       <c r="D9" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E9" s="10"/>
+      <c r="E9" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="F9" s="11"/>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
+      <c r="I9" s="10">
+        <v>2</v>
+      </c>
+      <c r="J9" s="10">
+        <v>1</v>
+      </c>
       <c r="K9" s="10"/>
       <c r="L9" s="11"/>
       <c r="M9" s="18" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="N9" s="10"/>
+      <c r="N9" s="21"/>
     </row>
     <row r="10" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="9"/>
+        <v>50</v>
+      </c>
+      <c r="C10" s="9">
+        <v>3</v>
+      </c>
       <c r="D10" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E10" s="10"/>
+      <c r="E10" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="F10" s="11"/>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
+      <c r="J10" s="10">
+        <v>1</v>
+      </c>
+      <c r="K10" s="10">
+        <v>2</v>
+      </c>
       <c r="L10" s="11"/>
       <c r="M10" s="18" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="N10" s="10"/>
+      <c r="N10" s="21"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>24</v>
       </c>
       <c r="C11" s="9">
         <v>2</v>
@@ -2015,7 +2211,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="10"/>
@@ -2030,558 +2226,1286 @@
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="N11" s="10"/>
+      <c r="N11" s="21"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="9">
         <v>2</v>
       </c>
       <c r="D12" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E12" s="10"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>58</v>
+      </c>
       <c r="F12" s="11"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
+      <c r="J12" s="10">
+        <v>2</v>
+      </c>
       <c r="K12" s="10"/>
       <c r="L12" s="11"/>
       <c r="M12" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-      <c r="N12" s="10"/>
-    </row>
-    <row r="13" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="9">
-        <v>2</v>
-      </c>
-      <c r="D13" s="9">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="18" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-      <c r="N13" s="10"/>
+        <v>Yes</v>
+      </c>
+      <c r="N12" s="21"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="35"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="21"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
-        <v>27</v>
+      <c r="A14" s="23" t="s">
+        <v>25</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="C14" s="9">
         <v>2</v>
       </c>
       <c r="D14" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="11"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
+      <c r="I14" s="10">
+        <v>1</v>
+      </c>
+      <c r="J14" s="10">
+        <v>1</v>
+      </c>
       <c r="K14" s="10"/>
       <c r="L14" s="11"/>
       <c r="M14" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-      <c r="N14" s="10"/>
+        <v>Yes</v>
+      </c>
+      <c r="N14" s="21"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="8" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="C15" s="9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D15" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E15" s="10"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>60</v>
+      </c>
       <c r="F15" s="11"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
+      <c r="I15" s="10">
+        <v>4</v>
+      </c>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
       <c r="L15" s="11"/>
       <c r="M15" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-      <c r="N15" s="10"/>
+        <v>Yes</v>
+      </c>
+      <c r="N15" s="21"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
-        <v>28</v>
+      <c r="A16" s="23" t="s">
+        <v>26</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C16" s="9">
         <v>2</v>
       </c>
       <c r="D16" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E16" s="21"/>
+        <v>0</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="F16" s="11"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
+      <c r="H16" s="10">
+        <v>2</v>
+      </c>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
       <c r="L16" s="11"/>
       <c r="M16" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-      <c r="N16" s="10"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
+        <v>Yes</v>
+      </c>
+      <c r="N16" s="21"/>
+    </row>
+    <row r="17" spans="1:202" x14ac:dyDescent="0.25">
+      <c r="A17" s="23"/>
       <c r="B17" s="8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C17" s="9">
         <v>2</v>
       </c>
       <c r="D17" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E17" s="10"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>73</v>
+      </c>
       <c r="F17" s="11"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
+      <c r="H17" s="10">
+        <v>2</v>
+      </c>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
       <c r="K17" s="10"/>
       <c r="L17" s="11"/>
       <c r="M17" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-      <c r="N17" s="10"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
+        <v>Yes</v>
+      </c>
+      <c r="N17" s="21"/>
+    </row>
+    <row r="18" spans="1:202" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
+        <v>27</v>
+      </c>
       <c r="B18" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C18" s="9">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D18" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="10">
+        <v>2</v>
+      </c>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10">
+        <v>2</v>
+      </c>
+      <c r="K18" s="10">
         <v>1</v>
       </c>
-      <c r="H18" s="10">
-        <v>1</v>
-      </c>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
       <c r="L18" s="11"/>
       <c r="M18" s="18" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="N18" s="10"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
-      <c r="B19" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="13">
+      <c r="N18" s="21"/>
+    </row>
+    <row r="19" spans="1:202" x14ac:dyDescent="0.25">
+      <c r="A19" s="23"/>
+      <c r="B19" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="9">
         <v>2</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19" s="9">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="11"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="21">
         <v>2</v>
       </c>
-      <c r="E19" s="14"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="20" t="str">
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-      <c r="N19" s="10"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
-      <c r="B20" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="13">
+        <v>Yes</v>
+      </c>
+      <c r="N19" s="21"/>
+    </row>
+    <row r="20" spans="1:202" x14ac:dyDescent="0.25">
+      <c r="A20" s="23"/>
+      <c r="B20" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="9">
         <v>2</v>
       </c>
-      <c r="D20" s="13">
+      <c r="D20" s="9">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="11"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10">
         <v>2</v>
       </c>
-      <c r="E20" s="14"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="20" t="str">
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-      <c r="N20" s="10"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="27" t="s">
-        <v>36</v>
-      </c>
+        <v>Yes</v>
+      </c>
+      <c r="N20" s="21"/>
+    </row>
+    <row r="21" spans="1:202" x14ac:dyDescent="0.25">
+      <c r="A21" s="24"/>
       <c r="B21" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="13"/>
+        <v>33</v>
+      </c>
+      <c r="C21" s="13">
+        <v>2</v>
+      </c>
       <c r="D21" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E21" s="14"/>
+      <c r="E21" s="10" t="s">
+        <v>61</v>
+      </c>
       <c r="F21" s="15"/>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
+      <c r="J21" s="22">
+        <v>2</v>
+      </c>
       <c r="K21" s="14"/>
       <c r="L21" s="15"/>
       <c r="M21" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="N21" s="10"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="27" t="s">
-        <v>38</v>
-      </c>
+      <c r="N21" s="21"/>
+    </row>
+    <row r="22" spans="1:202" x14ac:dyDescent="0.25">
+      <c r="A22" s="24"/>
       <c r="B22" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="13"/>
+        <v>34</v>
+      </c>
+      <c r="C22" s="13">
+        <v>2</v>
+      </c>
       <c r="D22" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E22" s="14"/>
+      <c r="E22" s="10" t="s">
+        <v>61</v>
+      </c>
       <c r="F22" s="15"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
+      <c r="K22" s="14">
+        <v>2</v>
+      </c>
       <c r="L22" s="15"/>
       <c r="M22" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="N22" s="10"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="27" t="s">
-        <v>40</v>
+      <c r="N22" s="21"/>
+    </row>
+    <row r="23" spans="1:202" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
+        <v>35</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="13">
-        <v>2</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C23" s="13"/>
       <c r="D23" s="13">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>59</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E23" s="14"/>
       <c r="F23" s="15"/>
-      <c r="G23" s="14">
-        <v>1</v>
-      </c>
+      <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
       <c r="K23" s="14"/>
       <c r="L23" s="15"/>
-      <c r="M23" s="22" t="str">
+      <c r="M23" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="N23" s="21"/>
+    </row>
+    <row r="24" spans="1:202" x14ac:dyDescent="0.25">
+      <c r="A24" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="50">
+        <v>1</v>
+      </c>
+      <c r="D24" s="50">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E24" s="51"/>
+      <c r="F24" s="51"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="51"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="51"/>
+      <c r="L24" s="51"/>
+      <c r="M24" s="52" t="str">
         <f t="shared" si="1"/>
         <v>No</v>
       </c>
-      <c r="N23" s="10"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H24" s="14"/>
-      <c r="M24" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>Yes</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="1">
-        <v>3</v>
+      <c r="N24" s="21"/>
+    </row>
+    <row r="25" spans="1:202" x14ac:dyDescent="0.25">
+      <c r="A25" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="13">
+        <v>2</v>
       </c>
       <c r="D25" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E25" t="s">
-        <v>60</v>
-      </c>
-      <c r="G25">
+      <c r="E25" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" s="15"/>
+      <c r="G25" s="14">
         <v>1</v>
       </c>
-      <c r="H25">
-        <v>2</v>
-      </c>
+      <c r="H25" s="14">
+        <v>1</v>
+      </c>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="15"/>
       <c r="M25" s="22" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" s="13">
+      <c r="N25" s="41"/>
+    </row>
+    <row r="26" spans="1:202" x14ac:dyDescent="0.25">
+      <c r="A26" s="28"/>
+      <c r="B26" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="54">
+        <v>2</v>
+      </c>
+      <c r="D26" s="50">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M26" s="22" t="str">
+        <v>2</v>
+      </c>
+      <c r="E26" s="55"/>
+      <c r="F26" s="55"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="51"/>
+      <c r="I26" s="55"/>
+      <c r="J26" s="55"/>
+      <c r="K26" s="55"/>
+      <c r="L26" s="55"/>
+      <c r="M26" s="52" t="str">
         <f t="shared" si="1"/>
-        <v>Yes</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+        <v>No</v>
+      </c>
+    </row>
+    <row r="27" spans="1:202" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="B27" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
+      </c>
+      <c r="C27" s="1">
+        <v>3</v>
       </c>
       <c r="D27" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M27" s="22" t="str">
+      <c r="E27" t="s">
+        <v>59</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>2</v>
+      </c>
+      <c r="M27" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>47</v>
-      </c>
+    <row r="28" spans="1:202" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="1">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="D28" s="13">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>59</v>
+      </c>
+      <c r="M28" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="29" spans="1:202" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="1">
+        <v>2</v>
+      </c>
+      <c r="D29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>60</v>
+      </c>
+      <c r="J29">
+        <v>2</v>
+      </c>
+      <c r="M29" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="30" spans="1:202" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="31"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="33"/>
+      <c r="M30" s="40"/>
+      <c r="N30" s="30"/>
+      <c r="O30" s="30"/>
+      <c r="P30" s="30"/>
+      <c r="Q30" s="30"/>
+      <c r="R30" s="30"/>
+      <c r="S30" s="30"/>
+      <c r="T30" s="30"/>
+      <c r="U30" s="30"/>
+      <c r="V30" s="30"/>
+      <c r="W30" s="30"/>
+      <c r="X30" s="30"/>
+      <c r="Y30" s="30"/>
+      <c r="Z30" s="30"/>
+      <c r="AA30" s="30"/>
+      <c r="AB30" s="30"/>
+      <c r="AC30" s="30"/>
+      <c r="AD30" s="30"/>
+      <c r="AE30" s="30"/>
+      <c r="AF30" s="30"/>
+      <c r="AG30" s="30"/>
+      <c r="AH30" s="30"/>
+      <c r="AI30" s="30"/>
+      <c r="AJ30" s="30"/>
+      <c r="AK30" s="30"/>
+      <c r="AL30" s="30"/>
+      <c r="AM30" s="30"/>
+      <c r="AN30" s="30"/>
+      <c r="AO30" s="30"/>
+      <c r="AP30" s="30"/>
+      <c r="AQ30" s="30"/>
+      <c r="AR30" s="30"/>
+      <c r="AS30" s="30"/>
+      <c r="AT30" s="30"/>
+      <c r="AU30" s="30"/>
+      <c r="AV30" s="30"/>
+      <c r="AW30" s="30"/>
+      <c r="AX30" s="30"/>
+      <c r="AY30" s="30"/>
+      <c r="AZ30" s="30"/>
+      <c r="BA30" s="30"/>
+      <c r="BB30" s="30"/>
+      <c r="BC30" s="30"/>
+      <c r="BD30" s="30"/>
+      <c r="BE30" s="30"/>
+      <c r="BF30" s="30"/>
+      <c r="BG30" s="30"/>
+      <c r="BH30" s="30"/>
+      <c r="BI30" s="30"/>
+      <c r="BJ30" s="30"/>
+      <c r="BK30" s="30"/>
+      <c r="BL30" s="30"/>
+      <c r="BM30" s="30"/>
+      <c r="BN30" s="30"/>
+      <c r="BO30" s="30"/>
+      <c r="BP30" s="30"/>
+      <c r="BQ30" s="30"/>
+      <c r="BR30" s="30"/>
+      <c r="BS30" s="30"/>
+      <c r="BT30" s="30"/>
+      <c r="BU30" s="30"/>
+      <c r="BV30" s="30"/>
+      <c r="BW30" s="30"/>
+      <c r="BX30" s="30"/>
+      <c r="BY30" s="30"/>
+      <c r="BZ30" s="30"/>
+      <c r="CA30" s="30"/>
+      <c r="CB30" s="30"/>
+      <c r="CC30" s="30"/>
+      <c r="CD30" s="30"/>
+      <c r="CE30" s="30"/>
+      <c r="CF30" s="30"/>
+      <c r="CG30" s="30"/>
+      <c r="CH30" s="30"/>
+      <c r="CI30" s="30"/>
+      <c r="CJ30" s="30"/>
+      <c r="CK30" s="30"/>
+      <c r="CL30" s="30"/>
+      <c r="CM30" s="30"/>
+      <c r="CN30" s="30"/>
+      <c r="CO30" s="30"/>
+      <c r="CP30" s="30"/>
+      <c r="CQ30" s="30"/>
+      <c r="CR30" s="30"/>
+      <c r="CS30" s="30"/>
+      <c r="CT30" s="30"/>
+      <c r="CU30" s="30"/>
+      <c r="CV30" s="30"/>
+      <c r="CW30" s="30"/>
+      <c r="CX30" s="30"/>
+      <c r="CY30" s="30"/>
+      <c r="CZ30" s="30"/>
+      <c r="DA30" s="30"/>
+      <c r="DB30" s="30"/>
+      <c r="DC30" s="30"/>
+      <c r="DD30" s="30"/>
+      <c r="DE30" s="30"/>
+      <c r="DF30" s="30"/>
+      <c r="DG30" s="30"/>
+      <c r="DH30" s="30"/>
+      <c r="DI30" s="30"/>
+      <c r="DJ30" s="30"/>
+      <c r="DK30" s="30"/>
+      <c r="DL30" s="30"/>
+      <c r="DM30" s="30"/>
+      <c r="DN30" s="30"/>
+      <c r="DO30" s="30"/>
+      <c r="DP30" s="30"/>
+      <c r="DQ30" s="30"/>
+      <c r="DR30" s="30"/>
+      <c r="DS30" s="30"/>
+      <c r="DT30" s="30"/>
+      <c r="DU30" s="30"/>
+      <c r="DV30" s="30"/>
+      <c r="DW30" s="30"/>
+      <c r="DX30" s="30"/>
+      <c r="DY30" s="30"/>
+      <c r="DZ30" s="30"/>
+      <c r="EA30" s="30"/>
+      <c r="EB30" s="30"/>
+      <c r="EC30" s="30"/>
+      <c r="ED30" s="30"/>
+      <c r="EE30" s="30"/>
+      <c r="EF30" s="30"/>
+      <c r="EG30" s="30"/>
+      <c r="EH30" s="30"/>
+      <c r="EI30" s="30"/>
+      <c r="EJ30" s="30"/>
+      <c r="EK30" s="30"/>
+      <c r="EL30" s="30"/>
+      <c r="EM30" s="30"/>
+      <c r="EN30" s="30"/>
+      <c r="EO30" s="30"/>
+      <c r="EP30" s="30"/>
+      <c r="EQ30" s="30"/>
+      <c r="ER30" s="30"/>
+      <c r="ES30" s="30"/>
+      <c r="ET30" s="30"/>
+      <c r="EU30" s="30"/>
+      <c r="EV30" s="30"/>
+      <c r="EW30" s="30"/>
+      <c r="EX30" s="30"/>
+      <c r="EY30" s="30"/>
+      <c r="EZ30" s="30"/>
+      <c r="FA30" s="30"/>
+      <c r="FB30" s="30"/>
+      <c r="FC30" s="30"/>
+      <c r="FD30" s="30"/>
+      <c r="FE30" s="30"/>
+      <c r="FF30" s="30"/>
+      <c r="FG30" s="30"/>
+      <c r="FH30" s="30"/>
+      <c r="FI30" s="30"/>
+      <c r="FJ30" s="30"/>
+      <c r="FK30" s="30"/>
+      <c r="FL30" s="30"/>
+      <c r="FM30" s="30"/>
+      <c r="FN30" s="30"/>
+      <c r="FO30" s="30"/>
+      <c r="FP30" s="30"/>
+      <c r="FQ30" s="30"/>
+      <c r="FR30" s="30"/>
+      <c r="FS30" s="30"/>
+      <c r="FT30" s="30"/>
+      <c r="FU30" s="30"/>
+      <c r="FV30" s="30"/>
+      <c r="FW30" s="30"/>
+      <c r="FX30" s="30"/>
+      <c r="FY30" s="30"/>
+      <c r="FZ30" s="30"/>
+      <c r="GA30" s="30"/>
+      <c r="GB30" s="30"/>
+      <c r="GC30" s="30"/>
+      <c r="GD30" s="30"/>
+      <c r="GE30" s="30"/>
+      <c r="GF30" s="30"/>
+      <c r="GG30" s="30"/>
+      <c r="GH30" s="30"/>
+      <c r="GI30" s="30"/>
+      <c r="GJ30" s="30"/>
+      <c r="GK30" s="30"/>
+      <c r="GL30" s="30"/>
+      <c r="GM30" s="30"/>
+      <c r="GN30" s="30"/>
+      <c r="GO30" s="30"/>
+      <c r="GP30" s="30"/>
+      <c r="GQ30" s="30"/>
+      <c r="GR30" s="30"/>
+      <c r="GS30" s="30"/>
+      <c r="GT30" s="30"/>
+    </row>
+    <row r="31" spans="1:202" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="1">
+        <v>4</v>
+      </c>
+      <c r="D31" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
+        <v>60</v>
+      </c>
+      <c r="G31">
         <v>1</v>
       </c>
-      <c r="E28" t="s">
-        <v>61</v>
-      </c>
-      <c r="G28">
-        <v>1</v>
-      </c>
-      <c r="H28">
-        <v>2</v>
-      </c>
-      <c r="M28" s="22" t="str">
+      <c r="H31">
+        <v>3</v>
+      </c>
+      <c r="M31" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="32" spans="1:202" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M32" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="33" spans="1:202" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="53" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" s="54">
+        <v>5</v>
+      </c>
+      <c r="D33" s="50">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E33" s="55"/>
+      <c r="F33" s="55"/>
+      <c r="G33" s="55"/>
+      <c r="H33" s="55"/>
+      <c r="I33" s="55"/>
+      <c r="J33" s="55"/>
+      <c r="K33" s="55"/>
+      <c r="L33" s="55"/>
+      <c r="M33" s="52" t="str">
         <f t="shared" si="1"/>
         <v>No</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D29" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M29" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>Yes</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" s="3" t="s">
+      <c r="N33" s="30"/>
+      <c r="O33" s="30"/>
+      <c r="P33" s="30"/>
+      <c r="Q33" s="30"/>
+      <c r="R33" s="30"/>
+      <c r="S33" s="30"/>
+      <c r="T33" s="30"/>
+      <c r="U33" s="30"/>
+      <c r="V33" s="30"/>
+      <c r="W33" s="30"/>
+      <c r="X33" s="30"/>
+      <c r="Y33" s="30"/>
+      <c r="Z33" s="30"/>
+      <c r="AA33" s="30"/>
+      <c r="AB33" s="30"/>
+      <c r="AC33" s="30"/>
+      <c r="AD33" s="30"/>
+      <c r="AE33" s="30"/>
+      <c r="AF33" s="30"/>
+      <c r="AG33" s="30"/>
+      <c r="AH33" s="30"/>
+      <c r="AI33" s="30"/>
+      <c r="AJ33" s="30"/>
+      <c r="AK33" s="30"/>
+      <c r="AL33" s="30"/>
+      <c r="AM33" s="30"/>
+      <c r="AN33" s="30"/>
+      <c r="AO33" s="30"/>
+      <c r="AP33" s="30"/>
+      <c r="AQ33" s="30"/>
+      <c r="AR33" s="30"/>
+      <c r="AS33" s="30"/>
+      <c r="AT33" s="30"/>
+      <c r="AU33" s="30"/>
+      <c r="AV33" s="30"/>
+      <c r="AW33" s="30"/>
+      <c r="AX33" s="30"/>
+      <c r="AY33" s="30"/>
+      <c r="AZ33" s="30"/>
+      <c r="BA33" s="30"/>
+      <c r="BB33" s="30"/>
+      <c r="BC33" s="30"/>
+      <c r="BD33" s="30"/>
+      <c r="BE33" s="30"/>
+      <c r="BF33" s="30"/>
+      <c r="BG33" s="30"/>
+      <c r="BH33" s="30"/>
+      <c r="BI33" s="30"/>
+      <c r="BJ33" s="30"/>
+      <c r="BK33" s="30"/>
+      <c r="BL33" s="30"/>
+      <c r="BM33" s="30"/>
+      <c r="BN33" s="30"/>
+      <c r="BO33" s="30"/>
+      <c r="BP33" s="30"/>
+      <c r="BQ33" s="30"/>
+      <c r="BR33" s="30"/>
+      <c r="BS33" s="30"/>
+      <c r="BT33" s="30"/>
+      <c r="BU33" s="30"/>
+      <c r="BV33" s="30"/>
+      <c r="BW33" s="30"/>
+      <c r="BX33" s="30"/>
+      <c r="BY33" s="30"/>
+      <c r="BZ33" s="30"/>
+      <c r="CA33" s="30"/>
+      <c r="CB33" s="30"/>
+      <c r="CC33" s="30"/>
+      <c r="CD33" s="30"/>
+      <c r="CE33" s="30"/>
+      <c r="CF33" s="30"/>
+      <c r="CG33" s="30"/>
+      <c r="CH33" s="30"/>
+      <c r="CI33" s="30"/>
+      <c r="CJ33" s="30"/>
+      <c r="CK33" s="30"/>
+      <c r="CL33" s="30"/>
+      <c r="CM33" s="30"/>
+      <c r="CN33" s="30"/>
+      <c r="CO33" s="30"/>
+      <c r="CP33" s="30"/>
+      <c r="CQ33" s="30"/>
+      <c r="CR33" s="30"/>
+      <c r="CS33" s="30"/>
+      <c r="CT33" s="30"/>
+      <c r="CU33" s="30"/>
+      <c r="CV33" s="30"/>
+      <c r="CW33" s="30"/>
+      <c r="CX33" s="30"/>
+      <c r="CY33" s="30"/>
+      <c r="CZ33" s="30"/>
+      <c r="DA33" s="30"/>
+      <c r="DB33" s="30"/>
+      <c r="DC33" s="30"/>
+      <c r="DD33" s="30"/>
+      <c r="DE33" s="30"/>
+      <c r="DF33" s="30"/>
+      <c r="DG33" s="30"/>
+      <c r="DH33" s="30"/>
+      <c r="DI33" s="30"/>
+      <c r="DJ33" s="30"/>
+      <c r="DK33" s="30"/>
+      <c r="DL33" s="30"/>
+      <c r="DM33" s="30"/>
+      <c r="DN33" s="30"/>
+      <c r="DO33" s="30"/>
+      <c r="DP33" s="30"/>
+      <c r="DQ33" s="30"/>
+      <c r="DR33" s="30"/>
+      <c r="DS33" s="30"/>
+      <c r="DT33" s="30"/>
+      <c r="DU33" s="30"/>
+      <c r="DV33" s="30"/>
+      <c r="DW33" s="30"/>
+      <c r="DX33" s="30"/>
+      <c r="DY33" s="30"/>
+      <c r="DZ33" s="30"/>
+      <c r="EA33" s="30"/>
+      <c r="EB33" s="30"/>
+      <c r="EC33" s="30"/>
+      <c r="ED33" s="30"/>
+      <c r="EE33" s="30"/>
+      <c r="EF33" s="30"/>
+      <c r="EG33" s="30"/>
+      <c r="EH33" s="30"/>
+      <c r="EI33" s="30"/>
+      <c r="EJ33" s="30"/>
+      <c r="EK33" s="30"/>
+      <c r="EL33" s="30"/>
+      <c r="EM33" s="30"/>
+      <c r="EN33" s="30"/>
+      <c r="EO33" s="30"/>
+      <c r="EP33" s="30"/>
+      <c r="EQ33" s="30"/>
+      <c r="ER33" s="30"/>
+      <c r="ES33" s="30"/>
+      <c r="ET33" s="30"/>
+      <c r="EU33" s="30"/>
+      <c r="EV33" s="30"/>
+      <c r="EW33" s="30"/>
+      <c r="EX33" s="30"/>
+      <c r="EY33" s="30"/>
+      <c r="EZ33" s="30"/>
+      <c r="FA33" s="30"/>
+      <c r="FB33" s="30"/>
+      <c r="FC33" s="30"/>
+      <c r="FD33" s="30"/>
+      <c r="FE33" s="30"/>
+      <c r="FF33" s="30"/>
+      <c r="FG33" s="30"/>
+      <c r="FH33" s="30"/>
+      <c r="FI33" s="30"/>
+      <c r="FJ33" s="30"/>
+      <c r="FK33" s="30"/>
+      <c r="FL33" s="30"/>
+      <c r="FM33" s="30"/>
+      <c r="FN33" s="30"/>
+      <c r="FO33" s="30"/>
+      <c r="FP33" s="30"/>
+      <c r="FQ33" s="30"/>
+      <c r="FR33" s="30"/>
+      <c r="FS33" s="30"/>
+      <c r="FT33" s="30"/>
+      <c r="FU33" s="30"/>
+      <c r="FV33" s="30"/>
+      <c r="FW33" s="30"/>
+      <c r="FX33" s="30"/>
+      <c r="FY33" s="30"/>
+      <c r="FZ33" s="30"/>
+      <c r="GA33" s="30"/>
+      <c r="GB33" s="30"/>
+      <c r="GC33" s="30"/>
+      <c r="GD33" s="30"/>
+      <c r="GE33" s="30"/>
+      <c r="GF33" s="30"/>
+      <c r="GG33" s="30"/>
+      <c r="GH33" s="30"/>
+      <c r="GI33" s="30"/>
+      <c r="GJ33" s="30"/>
+      <c r="GK33" s="30"/>
+      <c r="GL33" s="30"/>
+      <c r="GM33" s="30"/>
+      <c r="GN33" s="30"/>
+      <c r="GO33" s="30"/>
+      <c r="GP33" s="30"/>
+      <c r="GQ33" s="30"/>
+      <c r="GR33" s="30"/>
+      <c r="GS33" s="30"/>
+      <c r="GT33" s="30"/>
+    </row>
+    <row r="34" spans="1:202" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="53"/>
+      <c r="B34" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M30" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>Yes</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D31" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M31" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>Yes</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D32" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M32" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>Yes</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="1">
+      <c r="C34" s="54">
         <v>5</v>
       </c>
-      <c r="D33" s="13">
+      <c r="D34" s="50">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E33" t="s">
-        <v>66</v>
-      </c>
-      <c r="M33" s="22" t="str">
+      <c r="E34" s="55"/>
+      <c r="F34" s="55"/>
+      <c r="G34" s="55"/>
+      <c r="H34" s="55"/>
+      <c r="I34" s="55"/>
+      <c r="J34" s="55"/>
+      <c r="K34" s="55"/>
+      <c r="L34" s="55"/>
+      <c r="M34" s="52" t="str">
         <f t="shared" si="1"/>
         <v>No</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B34" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34" s="1">
-        <v>10</v>
-      </c>
-      <c r="D34" s="13">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="E34" t="s">
-        <v>61</v>
-      </c>
-      <c r="M34" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N34" s="30"/>
+      <c r="O34" s="30"/>
+      <c r="P34" s="30"/>
+      <c r="Q34" s="30"/>
+      <c r="R34" s="30"/>
+      <c r="S34" s="30"/>
+      <c r="T34" s="30"/>
+      <c r="U34" s="30"/>
+      <c r="V34" s="30"/>
+      <c r="W34" s="30"/>
+      <c r="X34" s="30"/>
+      <c r="Y34" s="30"/>
+      <c r="Z34" s="30"/>
+      <c r="AA34" s="30"/>
+      <c r="AB34" s="30"/>
+      <c r="AC34" s="30"/>
+      <c r="AD34" s="30"/>
+      <c r="AE34" s="30"/>
+      <c r="AF34" s="30"/>
+      <c r="AG34" s="30"/>
+      <c r="AH34" s="30"/>
+      <c r="AI34" s="30"/>
+      <c r="AJ34" s="30"/>
+      <c r="AK34" s="30"/>
+      <c r="AL34" s="30"/>
+      <c r="AM34" s="30"/>
+      <c r="AN34" s="30"/>
+      <c r="AO34" s="30"/>
+      <c r="AP34" s="30"/>
+      <c r="AQ34" s="30"/>
+      <c r="AR34" s="30"/>
+      <c r="AS34" s="30"/>
+      <c r="AT34" s="30"/>
+      <c r="AU34" s="30"/>
+      <c r="AV34" s="30"/>
+      <c r="AW34" s="30"/>
+      <c r="AX34" s="30"/>
+      <c r="AY34" s="30"/>
+      <c r="AZ34" s="30"/>
+      <c r="BA34" s="30"/>
+      <c r="BB34" s="30"/>
+      <c r="BC34" s="30"/>
+      <c r="BD34" s="30"/>
+      <c r="BE34" s="30"/>
+      <c r="BF34" s="30"/>
+      <c r="BG34" s="30"/>
+      <c r="BH34" s="30"/>
+      <c r="BI34" s="30"/>
+      <c r="BJ34" s="30"/>
+      <c r="BK34" s="30"/>
+      <c r="BL34" s="30"/>
+      <c r="BM34" s="30"/>
+      <c r="BN34" s="30"/>
+      <c r="BO34" s="30"/>
+      <c r="BP34" s="30"/>
+      <c r="BQ34" s="30"/>
+      <c r="BR34" s="30"/>
+      <c r="BS34" s="30"/>
+      <c r="BT34" s="30"/>
+      <c r="BU34" s="30"/>
+      <c r="BV34" s="30"/>
+      <c r="BW34" s="30"/>
+      <c r="BX34" s="30"/>
+      <c r="BY34" s="30"/>
+      <c r="BZ34" s="30"/>
+      <c r="CA34" s="30"/>
+      <c r="CB34" s="30"/>
+      <c r="CC34" s="30"/>
+      <c r="CD34" s="30"/>
+      <c r="CE34" s="30"/>
+      <c r="CF34" s="30"/>
+      <c r="CG34" s="30"/>
+      <c r="CH34" s="30"/>
+      <c r="CI34" s="30"/>
+      <c r="CJ34" s="30"/>
+      <c r="CK34" s="30"/>
+      <c r="CL34" s="30"/>
+      <c r="CM34" s="30"/>
+      <c r="CN34" s="30"/>
+      <c r="CO34" s="30"/>
+      <c r="CP34" s="30"/>
+      <c r="CQ34" s="30"/>
+      <c r="CR34" s="30"/>
+      <c r="CS34" s="30"/>
+      <c r="CT34" s="30"/>
+      <c r="CU34" s="30"/>
+      <c r="CV34" s="30"/>
+      <c r="CW34" s="30"/>
+      <c r="CX34" s="30"/>
+      <c r="CY34" s="30"/>
+      <c r="CZ34" s="30"/>
+      <c r="DA34" s="30"/>
+      <c r="DB34" s="30"/>
+      <c r="DC34" s="30"/>
+      <c r="DD34" s="30"/>
+      <c r="DE34" s="30"/>
+      <c r="DF34" s="30"/>
+      <c r="DG34" s="30"/>
+      <c r="DH34" s="30"/>
+      <c r="DI34" s="30"/>
+      <c r="DJ34" s="30"/>
+      <c r="DK34" s="30"/>
+      <c r="DL34" s="30"/>
+      <c r="DM34" s="30"/>
+      <c r="DN34" s="30"/>
+      <c r="DO34" s="30"/>
+      <c r="DP34" s="30"/>
+      <c r="DQ34" s="30"/>
+      <c r="DR34" s="30"/>
+      <c r="DS34" s="30"/>
+      <c r="DT34" s="30"/>
+      <c r="DU34" s="30"/>
+      <c r="DV34" s="30"/>
+      <c r="DW34" s="30"/>
+      <c r="DX34" s="30"/>
+      <c r="DY34" s="30"/>
+      <c r="DZ34" s="30"/>
+      <c r="EA34" s="30"/>
+      <c r="EB34" s="30"/>
+      <c r="EC34" s="30"/>
+      <c r="ED34" s="30"/>
+      <c r="EE34" s="30"/>
+      <c r="EF34" s="30"/>
+      <c r="EG34" s="30"/>
+      <c r="EH34" s="30"/>
+      <c r="EI34" s="30"/>
+      <c r="EJ34" s="30"/>
+      <c r="EK34" s="30"/>
+      <c r="EL34" s="30"/>
+      <c r="EM34" s="30"/>
+      <c r="EN34" s="30"/>
+      <c r="EO34" s="30"/>
+      <c r="EP34" s="30"/>
+      <c r="EQ34" s="30"/>
+      <c r="ER34" s="30"/>
+      <c r="ES34" s="30"/>
+      <c r="ET34" s="30"/>
+      <c r="EU34" s="30"/>
+      <c r="EV34" s="30"/>
+      <c r="EW34" s="30"/>
+      <c r="EX34" s="30"/>
+      <c r="EY34" s="30"/>
+      <c r="EZ34" s="30"/>
+      <c r="FA34" s="30"/>
+      <c r="FB34" s="30"/>
+      <c r="FC34" s="30"/>
+      <c r="FD34" s="30"/>
+      <c r="FE34" s="30"/>
+      <c r="FF34" s="30"/>
+      <c r="FG34" s="30"/>
+      <c r="FH34" s="30"/>
+      <c r="FI34" s="30"/>
+      <c r="FJ34" s="30"/>
+      <c r="FK34" s="30"/>
+      <c r="FL34" s="30"/>
+      <c r="FM34" s="30"/>
+      <c r="FN34" s="30"/>
+      <c r="FO34" s="30"/>
+      <c r="FP34" s="30"/>
+      <c r="FQ34" s="30"/>
+      <c r="FR34" s="30"/>
+      <c r="FS34" s="30"/>
+      <c r="FT34" s="30"/>
+      <c r="FU34" s="30"/>
+      <c r="FV34" s="30"/>
+      <c r="FW34" s="30"/>
+      <c r="FX34" s="30"/>
+      <c r="FY34" s="30"/>
+      <c r="FZ34" s="30"/>
+      <c r="GA34" s="30"/>
+      <c r="GB34" s="30"/>
+      <c r="GC34" s="30"/>
+      <c r="GD34" s="30"/>
+      <c r="GE34" s="30"/>
+      <c r="GF34" s="30"/>
+      <c r="GG34" s="30"/>
+      <c r="GH34" s="30"/>
+      <c r="GI34" s="30"/>
+      <c r="GJ34" s="30"/>
+      <c r="GK34" s="30"/>
+      <c r="GL34" s="30"/>
+      <c r="GM34" s="30"/>
+      <c r="GN34" s="30"/>
+      <c r="GO34" s="30"/>
+      <c r="GP34" s="30"/>
+      <c r="GQ34" s="30"/>
+      <c r="GR34" s="30"/>
+      <c r="GS34" s="30"/>
+      <c r="GT34" s="30"/>
+    </row>
+    <row r="35" spans="1:202" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="1">
+        <v>3</v>
+      </c>
       <c r="D35" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M35" s="22" t="str">
+      <c r="E35" t="s">
+        <v>65</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="K35">
+        <v>2</v>
+      </c>
+      <c r="M35" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:202" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C36" s="1">
+        <v>5</v>
+      </c>
       <c r="D36" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M36" s="22" t="str">
+      <c r="E36" t="s">
+        <v>65</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="M36" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D37" s="13">
+    <row r="37" spans="1:202" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="42"/>
+      <c r="B37" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="43">
+        <v>10</v>
+      </c>
+      <c r="D37" s="44">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M37" s="22" t="str">
+      <c r="E37" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="F37" s="46"/>
+      <c r="G37" s="45">
+        <v>2</v>
+      </c>
+      <c r="H37" s="45">
+        <v>1</v>
+      </c>
+      <c r="I37" s="45">
+        <v>2</v>
+      </c>
+      <c r="J37" s="45">
+        <v>2</v>
+      </c>
+      <c r="K37" s="45">
+        <v>3</v>
+      </c>
+      <c r="L37" s="46"/>
+      <c r="M37" s="47" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:202" x14ac:dyDescent="0.25">
       <c r="D38" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2591,7 +3515,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:202" x14ac:dyDescent="0.25">
       <c r="D39" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2601,7 +3525,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:202" x14ac:dyDescent="0.25">
       <c r="D40" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2611,7 +3535,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:202" x14ac:dyDescent="0.25">
       <c r="D41" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2621,7 +3545,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:202" x14ac:dyDescent="0.25">
       <c r="D42" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2631,7 +3555,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:202" x14ac:dyDescent="0.25">
       <c r="D43" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2641,7 +3565,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:202" x14ac:dyDescent="0.25">
       <c r="D44" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2651,7 +3575,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:202" x14ac:dyDescent="0.25">
       <c r="D45" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2661,7 +3585,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:202" x14ac:dyDescent="0.25">
       <c r="D46" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2671,7 +3595,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:202" x14ac:dyDescent="0.25">
       <c r="D47" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2681,7 +3605,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:202" x14ac:dyDescent="0.25">
       <c r="D48" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2883,7 +3807,7 @@
     </row>
     <row r="68" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D68" s="13">
-        <f t="shared" ref="D68:D131" si="2">C68 - SUM(G68:K68)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M68" s="22" t="str">
@@ -2893,7 +3817,7 @@
     </row>
     <row r="69" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D69" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M69" s="22" t="str">
@@ -2903,21 +3827,21 @@
     </row>
     <row r="70" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D70" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M70" s="22" t="str">
-        <f t="shared" ref="M70:M133" si="3">IF(D70 = 0,"Yes","No")</f>
+        <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="71" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D71" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D71:D134" si="2">C71 - SUM(G71:K71)</f>
         <v>0</v>
       </c>
       <c r="M71" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
     </row>
@@ -2927,7 +3851,7 @@
         <v>0</v>
       </c>
       <c r="M72" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
     </row>
@@ -2937,7 +3861,7 @@
         <v>0</v>
       </c>
       <c r="M73" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="M73:M136" si="3">IF(D73 = 0,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -3523,7 +4447,7 @@
     </row>
     <row r="132" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D132" s="13">
-        <f t="shared" ref="D132:D195" si="4">C132 - SUM(G132:K132)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M132" s="22" t="str">
@@ -3533,7 +4457,7 @@
     </row>
     <row r="133" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D133" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M133" s="22" t="str">
@@ -3543,21 +4467,21 @@
     </row>
     <row r="134" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D134" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M134" s="22" t="str">
-        <f t="shared" ref="M134:M197" si="5">IF(D134 = 0,"Yes","No")</f>
+        <f t="shared" si="3"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="135" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D135" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="D135:D198" si="4">C135 - SUM(G135:K135)</f>
         <v>0</v>
       </c>
       <c r="M135" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>Yes</v>
       </c>
     </row>
@@ -3567,7 +4491,7 @@
         <v>0</v>
       </c>
       <c r="M136" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>Yes</v>
       </c>
     </row>
@@ -3577,7 +4501,7 @@
         <v>0</v>
       </c>
       <c r="M137" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="M137:M200" si="5">IF(D137 = 0,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -4163,7 +5087,7 @@
     </row>
     <row r="196" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D196" s="13">
-        <f t="shared" ref="D196:D259" si="6">C196 - SUM(G196:K196)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M196" s="22" t="str">
@@ -4173,7 +5097,7 @@
     </row>
     <row r="197" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D197" s="13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M197" s="22" t="str">
@@ -4183,21 +5107,21 @@
     </row>
     <row r="198" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D198" s="13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M198" s="22" t="str">
-        <f t="shared" ref="M198:M261" si="7">IF(D198 = 0,"Yes","No")</f>
+        <f t="shared" si="5"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="199" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D199" s="13">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="D199:D262" si="6">C199 - SUM(G199:K199)</f>
         <v>0</v>
       </c>
       <c r="M199" s="22" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>Yes</v>
       </c>
     </row>
@@ -4207,7 +5131,7 @@
         <v>0</v>
       </c>
       <c r="M200" s="22" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>Yes</v>
       </c>
     </row>
@@ -4217,7 +5141,7 @@
         <v>0</v>
       </c>
       <c r="M201" s="22" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="M201:M264" si="7">IF(D201 = 0,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -4803,7 +5727,7 @@
     </row>
     <row r="260" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D260" s="13">
-        <f t="shared" ref="D260:D323" si="8">C260 - SUM(G260:K260)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M260" s="22" t="str">
@@ -4813,7 +5737,7 @@
     </row>
     <row r="261" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D261" s="13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M261" s="22" t="str">
@@ -4823,21 +5747,21 @@
     </row>
     <row r="262" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D262" s="13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M262" s="22" t="str">
-        <f t="shared" ref="M262:M325" si="9">IF(D262 = 0,"Yes","No")</f>
+        <f t="shared" si="7"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="263" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D263" s="13">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="D263:D326" si="8">C263 - SUM(G263:K263)</f>
         <v>0</v>
       </c>
       <c r="M263" s="22" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>Yes</v>
       </c>
     </row>
@@ -4847,7 +5771,7 @@
         <v>0</v>
       </c>
       <c r="M264" s="22" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>Yes</v>
       </c>
     </row>
@@ -4857,7 +5781,7 @@
         <v>0</v>
       </c>
       <c r="M265" s="22" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="M265:M328" si="9">IF(D265 = 0,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -5443,7 +6367,7 @@
     </row>
     <row r="324" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D324" s="13">
-        <f t="shared" ref="D324:D387" si="10">C324 - SUM(G324:K324)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="M324" s="22" t="str">
@@ -5453,7 +6377,7 @@
     </row>
     <row r="325" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D325" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="M325" s="22" t="str">
@@ -5463,21 +6387,21 @@
     </row>
     <row r="326" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D326" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="M326" s="22" t="str">
-        <f t="shared" ref="M326:M389" si="11">IF(D326 = 0,"Yes","No")</f>
+        <f t="shared" si="9"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="327" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D327" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="D327:D390" si="10">C327 - SUM(G327:K327)</f>
         <v>0</v>
       </c>
       <c r="M327" s="22" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>Yes</v>
       </c>
     </row>
@@ -5487,7 +6411,7 @@
         <v>0</v>
       </c>
       <c r="M328" s="22" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>Yes</v>
       </c>
     </row>
@@ -5497,7 +6421,7 @@
         <v>0</v>
       </c>
       <c r="M329" s="22" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="M329:M392" si="11">IF(D329 = 0,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -6083,7 +7007,7 @@
     </row>
     <row r="388" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D388" s="13">
-        <f t="shared" ref="D388:D451" si="12">C388 - SUM(G388:K388)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="M388" s="22" t="str">
@@ -6093,7 +7017,7 @@
     </row>
     <row r="389" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D389" s="13">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="M389" s="22" t="str">
@@ -6103,21 +7027,21 @@
     </row>
     <row r="390" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D390" s="13">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="M390" s="22" t="str">
-        <f t="shared" ref="M390:M453" si="13">IF(D390 = 0,"Yes","No")</f>
+        <f t="shared" si="11"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="391" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D391" s="13">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="D391:D454" si="12">C391 - SUM(G391:K391)</f>
         <v>0</v>
       </c>
       <c r="M391" s="22" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>Yes</v>
       </c>
     </row>
@@ -6127,7 +7051,7 @@
         <v>0</v>
       </c>
       <c r="M392" s="22" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>Yes</v>
       </c>
     </row>
@@ -6137,7 +7061,7 @@
         <v>0</v>
       </c>
       <c r="M393" s="22" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="M393:M456" si="13">IF(D393 = 0,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -6723,7 +7647,7 @@
     </row>
     <row r="452" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D452" s="13">
-        <f t="shared" ref="D452:D515" si="14">C452 - SUM(G452:K452)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M452" s="22" t="str">
@@ -6733,7 +7657,7 @@
     </row>
     <row r="453" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D453" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M453" s="22" t="str">
@@ -6743,21 +7667,21 @@
     </row>
     <row r="454" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D454" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M454" s="22" t="str">
-        <f t="shared" ref="M454:M517" si="15">IF(D454 = 0,"Yes","No")</f>
+        <f t="shared" si="13"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="455" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D455" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="D455:D518" si="14">C455 - SUM(G455:K455)</f>
         <v>0</v>
       </c>
       <c r="M455" s="22" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>Yes</v>
       </c>
     </row>
@@ -6767,7 +7691,7 @@
         <v>0</v>
       </c>
       <c r="M456" s="22" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>Yes</v>
       </c>
     </row>
@@ -6777,7 +7701,7 @@
         <v>0</v>
       </c>
       <c r="M457" s="22" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="M457:M520" si="15">IF(D457 = 0,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -7363,7 +8287,7 @@
     </row>
     <row r="516" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D516" s="13">
-        <f t="shared" ref="D516:D579" si="16">C516 - SUM(G516:K516)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M516" s="22" t="str">
@@ -7373,7 +8297,7 @@
     </row>
     <row r="517" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D517" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M517" s="22" t="str">
@@ -7383,21 +8307,21 @@
     </row>
     <row r="518" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D518" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M518" s="22" t="str">
-        <f t="shared" ref="M518:M581" si="17">IF(D518 = 0,"Yes","No")</f>
+        <f t="shared" si="15"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="519" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D519" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="D519:D582" si="16">C519 - SUM(G519:K519)</f>
         <v>0</v>
       </c>
       <c r="M519" s="22" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Yes</v>
       </c>
     </row>
@@ -7407,7 +8331,7 @@
         <v>0</v>
       </c>
       <c r="M520" s="22" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Yes</v>
       </c>
     </row>
@@ -7417,7 +8341,7 @@
         <v>0</v>
       </c>
       <c r="M521" s="22" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="M521:M584" si="17">IF(D521 = 0,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -8003,7 +8927,7 @@
     </row>
     <row r="580" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D580" s="13">
-        <f t="shared" ref="D580:D643" si="18">C580 - SUM(G580:K580)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="M580" s="22" t="str">
@@ -8013,7 +8937,7 @@
     </row>
     <row r="581" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D581" s="13">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="M581" s="22" t="str">
@@ -8023,21 +8947,21 @@
     </row>
     <row r="582" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D582" s="13">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="M582" s="22" t="str">
-        <f t="shared" ref="M582:M645" si="19">IF(D582 = 0,"Yes","No")</f>
+        <f t="shared" si="17"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="583" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D583" s="13">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="D583:D646" si="18">C583 - SUM(G583:K583)</f>
         <v>0</v>
       </c>
       <c r="M583" s="22" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>Yes</v>
       </c>
     </row>
@@ -8047,7 +8971,7 @@
         <v>0</v>
       </c>
       <c r="M584" s="22" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>Yes</v>
       </c>
     </row>
@@ -8057,7 +8981,7 @@
         <v>0</v>
       </c>
       <c r="M585" s="22" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="M585:M648" si="19">IF(D585 = 0,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -8643,7 +9567,7 @@
     </row>
     <row r="644" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D644" s="13">
-        <f t="shared" ref="D644:D707" si="20">C644 - SUM(G644:K644)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="M644" s="22" t="str">
@@ -8653,7 +9577,7 @@
     </row>
     <row r="645" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D645" s="13">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="M645" s="22" t="str">
@@ -8663,21 +9587,21 @@
     </row>
     <row r="646" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D646" s="13">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="M646" s="22" t="str">
-        <f t="shared" ref="M646:M709" si="21">IF(D646 = 0,"Yes","No")</f>
+        <f t="shared" si="19"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="647" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D647" s="13">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="D647:D710" si="20">C647 - SUM(G647:K647)</f>
         <v>0</v>
       </c>
       <c r="M647" s="22" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>Yes</v>
       </c>
     </row>
@@ -8687,7 +9611,7 @@
         <v>0</v>
       </c>
       <c r="M648" s="22" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>Yes</v>
       </c>
     </row>
@@ -8697,7 +9621,7 @@
         <v>0</v>
       </c>
       <c r="M649" s="22" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="M649:M712" si="21">IF(D649 = 0,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -9283,7 +10207,7 @@
     </row>
     <row r="708" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D708" s="13">
-        <f t="shared" ref="D708:D771" si="22">C708 - SUM(G708:K708)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="M708" s="22" t="str">
@@ -9293,7 +10217,7 @@
     </row>
     <row r="709" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D709" s="13">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="M709" s="22" t="str">
@@ -9303,21 +10227,21 @@
     </row>
     <row r="710" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D710" s="13">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="M710" s="22" t="str">
-        <f t="shared" ref="M710:M773" si="23">IF(D710 = 0,"Yes","No")</f>
+        <f t="shared" si="21"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="711" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D711" s="13">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="D711:D774" si="22">C711 - SUM(G711:K711)</f>
         <v>0</v>
       </c>
       <c r="M711" s="22" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>Yes</v>
       </c>
     </row>
@@ -9327,7 +10251,7 @@
         <v>0</v>
       </c>
       <c r="M712" s="22" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>Yes</v>
       </c>
     </row>
@@ -9337,7 +10261,7 @@
         <v>0</v>
       </c>
       <c r="M713" s="22" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" ref="M713:M776" si="23">IF(D713 = 0,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -9923,7 +10847,7 @@
     </row>
     <row r="772" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D772" s="13">
-        <f t="shared" ref="D772:D835" si="24">C772 - SUM(G772:K772)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M772" s="22" t="str">
@@ -9933,7 +10857,7 @@
     </row>
     <row r="773" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D773" s="13">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M773" s="22" t="str">
@@ -9943,21 +10867,21 @@
     </row>
     <row r="774" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D774" s="13">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M774" s="22" t="str">
-        <f t="shared" ref="M774:M837" si="25">IF(D774 = 0,"Yes","No")</f>
+        <f t="shared" si="23"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="775" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D775" s="13">
-        <f t="shared" si="24"/>
+        <f t="shared" ref="D775:D838" si="24">C775 - SUM(G775:K775)</f>
         <v>0</v>
       </c>
       <c r="M775" s="22" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>Yes</v>
       </c>
     </row>
@@ -9967,7 +10891,7 @@
         <v>0</v>
       </c>
       <c r="M776" s="22" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>Yes</v>
       </c>
     </row>
@@ -9977,7 +10901,7 @@
         <v>0</v>
       </c>
       <c r="M777" s="22" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" ref="M777:M840" si="25">IF(D777 = 0,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -10563,7 +11487,7 @@
     </row>
     <row r="836" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D836" s="13">
-        <f t="shared" ref="D836:D899" si="26">C836 - SUM(G836:K836)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M836" s="22" t="str">
@@ -10573,7 +11497,7 @@
     </row>
     <row r="837" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D837" s="13">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M837" s="22" t="str">
@@ -10583,21 +11507,21 @@
     </row>
     <row r="838" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D838" s="13">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M838" s="22" t="str">
-        <f t="shared" ref="M838:M901" si="27">IF(D838 = 0,"Yes","No")</f>
+        <f t="shared" si="25"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="839" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D839" s="13">
-        <f t="shared" si="26"/>
+        <f t="shared" ref="D839:D902" si="26">C839 - SUM(G839:K839)</f>
         <v>0</v>
       </c>
       <c r="M839" s="22" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>Yes</v>
       </c>
     </row>
@@ -10607,7 +11531,7 @@
         <v>0</v>
       </c>
       <c r="M840" s="22" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>Yes</v>
       </c>
     </row>
@@ -10617,7 +11541,7 @@
         <v>0</v>
       </c>
       <c r="M841" s="22" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" ref="M841:M904" si="27">IF(D841 = 0,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -11203,7 +12127,7 @@
     </row>
     <row r="900" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D900" s="13">
-        <f t="shared" ref="D900:D963" si="28">C900 - SUM(G900:K900)</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="M900" s="22" t="str">
@@ -11213,7 +12137,7 @@
     </row>
     <row r="901" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D901" s="13">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="M901" s="22" t="str">
@@ -11223,21 +12147,21 @@
     </row>
     <row r="902" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D902" s="13">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="M902" s="22" t="str">
-        <f t="shared" ref="M902:M965" si="29">IF(D902 = 0,"Yes","No")</f>
+        <f t="shared" si="27"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="903" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D903" s="13">
-        <f t="shared" si="28"/>
+        <f t="shared" ref="D903:D966" si="28">C903 - SUM(G903:K903)</f>
         <v>0</v>
       </c>
       <c r="M903" s="22" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="27"/>
         <v>Yes</v>
       </c>
     </row>
@@ -11247,7 +12171,7 @@
         <v>0</v>
       </c>
       <c r="M904" s="22" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="27"/>
         <v>Yes</v>
       </c>
     </row>
@@ -11257,7 +12181,7 @@
         <v>0</v>
       </c>
       <c r="M905" s="22" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" ref="M905:M968" si="29">IF(D905 = 0,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -11843,7 +12767,7 @@
     </row>
     <row r="964" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D964" s="13">
-        <f t="shared" ref="D964:D1027" si="30">C964 - SUM(G964:K964)</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="M964" s="22" t="str">
@@ -11853,7 +12777,7 @@
     </row>
     <row r="965" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D965" s="13">
-        <f t="shared" si="30"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="M965" s="22" t="str">
@@ -11863,21 +12787,21 @@
     </row>
     <row r="966" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D966" s="13">
-        <f t="shared" si="30"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="M966" s="22" t="str">
-        <f t="shared" ref="M966:M1029" si="31">IF(D966 = 0,"Yes","No")</f>
+        <f t="shared" si="29"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="967" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D967" s="13">
-        <f t="shared" si="30"/>
+        <f t="shared" ref="D967:D1030" si="30">C967 - SUM(G967:K967)</f>
         <v>0</v>
       </c>
       <c r="M967" s="22" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="29"/>
         <v>Yes</v>
       </c>
     </row>
@@ -11887,7 +12811,7 @@
         <v>0</v>
       </c>
       <c r="M968" s="22" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="29"/>
         <v>Yes</v>
       </c>
     </row>
@@ -11897,7 +12821,7 @@
         <v>0</v>
       </c>
       <c r="M969" s="22" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" ref="M969:M1032" si="31">IF(D969 = 0,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -12483,7 +13407,7 @@
     </row>
     <row r="1028" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D1028" s="13">
-        <f t="shared" ref="D1028:D1091" si="32">C1028 - SUM(G1028:K1028)</f>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="M1028" s="22" t="str">
@@ -12493,7 +13417,7 @@
     </row>
     <row r="1029" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D1029" s="13">
-        <f t="shared" si="32"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="M1029" s="22" t="str">
@@ -12503,21 +13427,21 @@
     </row>
     <row r="1030" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D1030" s="13">
-        <f t="shared" si="32"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="M1030" s="22" t="str">
-        <f t="shared" ref="M1030:M1093" si="33">IF(D1030 = 0,"Yes","No")</f>
+        <f t="shared" si="31"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="1031" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D1031" s="13">
-        <f t="shared" si="32"/>
+        <f t="shared" ref="D1031:D1094" si="32">C1031 - SUM(G1031:K1031)</f>
         <v>0</v>
       </c>
       <c r="M1031" s="22" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>Yes</v>
       </c>
     </row>
@@ -12527,7 +13451,7 @@
         <v>0</v>
       </c>
       <c r="M1032" s="22" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>Yes</v>
       </c>
     </row>
@@ -12537,7 +13461,7 @@
         <v>0</v>
       </c>
       <c r="M1033" s="22" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" ref="M1033:M1096" si="33">IF(D1033 = 0,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -13123,7 +14047,7 @@
     </row>
     <row r="1092" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D1092" s="13">
-        <f t="shared" ref="D1092:D1155" si="34">C1092 - SUM(G1092:K1092)</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="M1092" s="22" t="str">
@@ -13133,7 +14057,7 @@
     </row>
     <row r="1093" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D1093" s="13">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="M1093" s="22" t="str">
@@ -13143,21 +14067,21 @@
     </row>
     <row r="1094" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D1094" s="13">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="M1094" s="22" t="str">
-        <f t="shared" ref="M1094:M1157" si="35">IF(D1094 = 0,"Yes","No")</f>
+        <f t="shared" si="33"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="1095" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D1095" s="13">
-        <f t="shared" si="34"/>
+        <f t="shared" ref="D1095:D1158" si="34">C1095 - SUM(G1095:K1095)</f>
         <v>0</v>
       </c>
       <c r="M1095" s="22" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="33"/>
         <v>Yes</v>
       </c>
     </row>
@@ -13167,7 +14091,7 @@
         <v>0</v>
       </c>
       <c r="M1096" s="22" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="33"/>
         <v>Yes</v>
       </c>
     </row>
@@ -13177,7 +14101,7 @@
         <v>0</v>
       </c>
       <c r="M1097" s="22" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" ref="M1097:M1160" si="35">IF(D1097 = 0,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -13763,7 +14687,7 @@
     </row>
     <row r="1156" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D1156" s="13">
-        <f t="shared" ref="D1156:D1219" si="36">C1156 - SUM(G1156:K1156)</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="M1156" s="22" t="str">
@@ -13773,7 +14697,7 @@
     </row>
     <row r="1157" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D1157" s="13">
-        <f t="shared" si="36"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="M1157" s="22" t="str">
@@ -13783,21 +14707,21 @@
     </row>
     <row r="1158" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D1158" s="13">
-        <f t="shared" si="36"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="M1158" s="22" t="str">
-        <f t="shared" ref="M1158:M1221" si="37">IF(D1158 = 0,"Yes","No")</f>
+        <f t="shared" si="35"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="1159" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D1159" s="13">
-        <f t="shared" si="36"/>
+        <f t="shared" ref="D1159:D1222" si="36">C1159 - SUM(G1159:K1159)</f>
         <v>0</v>
       </c>
       <c r="M1159" s="22" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="35"/>
         <v>Yes</v>
       </c>
     </row>
@@ -13807,7 +14731,7 @@
         <v>0</v>
       </c>
       <c r="M1160" s="22" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="35"/>
         <v>Yes</v>
       </c>
     </row>
@@ -13817,7 +14741,7 @@
         <v>0</v>
       </c>
       <c r="M1161" s="22" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" ref="M1161:M1224" si="37">IF(D1161 = 0,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -14403,7 +15327,7 @@
     </row>
     <row r="1220" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D1220" s="13">
-        <f t="shared" ref="D1220:D1224" si="38">C1220 - SUM(G1220:K1220)</f>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="M1220" s="22" t="str">
@@ -14413,7 +15337,7 @@
     </row>
     <row r="1221" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D1221" s="13">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="M1221" s="22" t="str">
@@ -14423,21 +15347,21 @@
     </row>
     <row r="1222" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D1222" s="13">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="M1222" s="22" t="str">
-        <f t="shared" ref="M1222:M1224" si="39">IF(D1222 = 0,"Yes","No")</f>
+        <f t="shared" si="37"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="1223" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D1223" s="13">
-        <f t="shared" si="38"/>
+        <f t="shared" ref="D1223:D1227" si="38">C1223 - SUM(G1223:K1223)</f>
         <v>0</v>
       </c>
       <c r="M1223" s="22" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="37"/>
         <v>Yes</v>
       </c>
     </row>
@@ -14447,6 +15371,36 @@
         <v>0</v>
       </c>
       <c r="M1224" s="22" t="str">
+        <f t="shared" si="37"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="1225" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D1225" s="13">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="M1225" s="22" t="str">
+        <f t="shared" ref="M1225:M1227" si="39">IF(D1225 = 0,"Yes","No")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="1226" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D1226" s="13">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="M1226" s="22" t="str">
+        <f t="shared" si="39"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="1227" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D1227" s="13">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="M1227" s="22" t="str">
         <f t="shared" si="39"/>
         <v>Yes</v>
       </c>
@@ -14541,31 +15495,31 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>SUM('Sprint 2 Backlog'!C:C)</f>
-        <v>46</v>
+        <v>96</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -14587,23 +15541,23 @@
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>$A$2 - SUM('Sprint 2 Backlog'!G:G)</f>
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="B6">
         <f>$A$2 - SUM('Sprint 2 Backlog'!G:H)</f>
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="C6">
         <f>$A$2 - SUM('Sprint 2 Backlog'!G:I)</f>
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="D6">
         <f>$A$2 - SUM('Sprint 2 Backlog'!G:J)</f>
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E6">
         <f>$A$2 - SUM('Sprint 2 Backlog'!G:K)</f>
-        <v>33</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>